<commit_message>
Updated scripts for VMware.PowerCLI->VCF.PowerCLI change.
</commit_message>
<xml_diff>
--- a/security-configuration-hardening-guide/vsan/8.0/VMware vSphere Security Configuration Guide 8 - Changes.xlsx
+++ b/security-configuration-hardening-guide/vsan/8.0/VMware vSphere Security Configuration Guide 8 - Changes.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28526"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28730"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{37779A1A-09FD-45D3-A2EC-095CC51E076B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{26E75665-BA94-4A45-A0F4-78712261DC91}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5250" yWindow="2715" windowWidth="32055" windowHeight="16950" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1395" yWindow="3750" windowWidth="45480" windowHeight="15030" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Introduction" sheetId="18" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3705" uniqueCount="1272">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3705" uniqueCount="1273">
   <si>
     <t>See the included documentation for important guidance and instructions.</t>
   </si>
@@ -4420,6 +4420,9 @@
   </si>
   <si>
     <t>Version 803-20250422-01</t>
+  </si>
+  <si>
+    <t>Version 803-20250709-01</t>
   </si>
 </sst>
 </file>
@@ -7481,9 +7484,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B983C5FE-A1EF-4EF9-9A3B-A256EFBEDC4C}">
   <dimension ref="A1:C9"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
-    </sheetView>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="38.140625" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
@@ -7500,7 +7501,7 @@
     </row>
     <row r="2" spans="1:1" ht="21" x14ac:dyDescent="0.25">
       <c r="A2" s="26" t="s">
-        <v>1271</v>
+        <v>1272</v>
       </c>
     </row>
     <row r="3" spans="1:1" ht="21" x14ac:dyDescent="0.25">

</xml_diff>